<commit_message>
Reformatting and re-structuring test case document with required test data
</commit_message>
<xml_diff>
--- a/Test Coverage/Test_Cases.xlsx
+++ b/Test Coverage/Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3886416\CSE Drive\Comcast\Repo\Fruit-Basket-App\Test Coverage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D98C077-C04A-484B-B536-21D694A6F3B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BB047D-AB5D-441B-B485-7FFEDEF7E384}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
   <si>
     <t>2. User need to have write &amp;execution permissions</t>
   </si>
@@ -51,14 +51,6 @@
   </si>
   <si>
     <t>Verify the file selection</t>
-  </si>
-  <si>
-    <t>Add a valid file in the expected valid path</t>
-  </si>
-  <si>
-    <t>1. Upload the CSV file to the server
-2.set the correct location for the variables call"filepath" and "filename"
-3. Execute the fruitbasketapp.sh script.</t>
   </si>
   <si>
     <t>https://github.com/Dasithz/Fruit-Basket-App/blob/master/test.csv</t>
@@ -144,43 +136,6 @@
     <t>""Exit Code : 2 ! Terminating the script due to the csv validation failure! CSV contains more or less fields than expected. Please check the test.csv file which located under /home/dasitha/""</t>
   </si>
   <si>
-    <t>Verify the file path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of fruits:
-21
-Total types of fruits:
-5
-Oldest fruit &amp; age:
-pineapple: 6
-orange: 6
-The number of each type of fruit in descending order:
-orange: 6
-apple: 5
-pineapple: 4
-grapefruit: 4
-watermelon: 3
-The various characteristics (count, color, shape, etc.) of each fruit by type:
-      1 apple: green, tart
-      3 apple: red, sweet
-      1 apple: yellow, sweet
-      2 grapefruit: bitter, yellow
-      2 grapefruit: yellow, bitter
-      5 orange: round, sweet
-      1 orange: sweet, round
-      2 pineapple: prickly, sweet
-      2 pineapple: sweet, prickly
-      1 watermelon: green, heavy
-      2 watermelon: heavy, green
-</t>
-  </si>
-  <si>
-    <t>Verify the CSV file content</t>
-  </si>
-  <si>
-    <t>Input file have all required columns according to the expected format.</t>
-  </si>
-  <si>
     <t>Input file doesn't have all required columns</t>
   </si>
   <si>
@@ -216,45 +171,7 @@
 </t>
   </si>
   <si>
-    <t>Add numbers only to the second column</t>
-  </si>
-  <si>
-    <t>1. Open the test.CSV file and 
-2. Change the second column data in the second raw to random numbers.
-3. Upload the file.
-4. Set the correct uploaded path to the "filepath" variable and set the file name to the "filename" variable.
-5 Execute the fruitbasketapp.sh script.</t>
-  </si>
-  <si>
     <t>https://github.com/Dasithz/Fruit-Basket-App/blob/master/Test%20Coverage/CSV_For_Test_Case_11.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of fruits:
-21
-Total types of fruits:
-5
-Oldest fruit &amp; age:
-pineapple: 6
-orange: 6
-The number of each type of fruit in descending order:
-orange: 6
-apple: 5
-pineapple: 4
-grapefruit: 4
-watermelon: 3
-The various characteristics (count, color, shape, etc.) of each fruit by type:
-      1 apple: green, tart
-      3 apple: red, sweet
-      1 apple: yellow, sweet
-      2 grapefruit: bitter, yellow
-      2 grapefruit: yellow, bitter
-      5 orange: round, sweet
-      1 orange: sweet, round
-      2 pineapple: prickly, sweet
-      2 pineapple: sweet, prickly
-      1 watermelon: green, heavy
-      2 watermelon: heavy, green
-</t>
   </si>
   <si>
     <t>Add numbers and letters to the second column</t>
@@ -318,13 +235,7 @@
 5 Execute the fruitbasketapp.sh script.</t>
   </si>
   <si>
-    <t>https://github.com/Dasithz/Fruit-Basket-App/blob/master/Test%20Coverage/CSV_For_Test_Case_16.csv</t>
-  </si>
-  <si>
     <t>Adding an extra column</t>
-  </si>
-  <si>
-    <t>https://github.com/Dasithz/Fruit-Basket-App/blob/master/Test%20Coverage/CSV_For_Test_Case_17.csv</t>
   </si>
   <si>
     <t>"Exit Code : 2 ! Terminating the script due to the csv validation failure! CSV contains more or less fields than expected. Please check the test.csv file which located under /home/dasitha/"</t>
@@ -341,9 +252,6 @@
 3. Upload the file.
 4. Set the correct uploaded path to the "filepath" variable and set the file name to the "filename" variable.
 5 Execute the fruitbasketapp.sh script.</t>
-  </si>
-  <si>
-    <t>https://github.com/Dasithz/Fruit-Basket-App/blob/master/Test%20Coverage/CSV_For_Test_Case_18.csv</t>
   </si>
   <si>
     <t xml:space="preserve"> Exit Code : 5 ! Terminating the script due to the csv validation failure! </t>
@@ -510,19 +418,6 @@
 4. Execute the fruitbasketapp.sh script.</t>
   </si>
   <si>
-    <t xml:space="preserve">
-1. Upload a file with required format to the server location
-2. initialize the file name to the variable "filename"
-3. initialize "filepath" variable in the script with the correct location.
-4. Execute the fruitbasketapp.sh script.</t>
-  </si>
-  <si>
-    <t>1. Navigate to the desired location which define in the "filepath" variable.
-2. Upload the CSV file with the required format. (String,Integer,String,String)
-3. Initialize the file name to the variable "filename"
-4. Execute the fruitbasketapp.sh script.</t>
-  </si>
-  <si>
     <t>Verify the validation of the first column in the CSV file</t>
   </si>
   <si>
@@ -530,9 +425,6 @@
   </si>
   <si>
     <t>Change the first columns to  numbers and characters</t>
-  </si>
-  <si>
-    <t>Verify the validation of th second column in the CSV file</t>
   </si>
   <si>
     <t>Verify the validation of the third column in the CSV file</t>
@@ -666,6 +558,20 @@
   <si>
     <t>Exit Code: 1 File test.csv does not exist in the give path &lt;filepath&gt; or no path defined. Terminating the script!</t>
   </si>
+  <si>
+    <t>1. Upload the CSV file to the server according to the correct format. (4 columns : (string,integer,string,string)
+2.Set the correct location to the "filepath" and exact file to the "filename" variable.
+3. Execute the fruitbasketapp.sh script.</t>
+  </si>
+  <si>
+    <t>https://github.com/Dasithz/Fruit-Basket-App/blob/master/Test%20Coverage/CSV_For_Test_Case_7.csv</t>
+  </si>
+  <si>
+    <t>https://github.com/Dasithz/Fruit-Basket-App/blob/master/Test%20Coverage/CSV_For_Test_Case_6.csv</t>
+  </si>
+  <si>
+    <t>Add a valid file to the expected valid path</t>
+  </si>
 </sst>
 </file>
 
@@ -690,12 +596,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -772,6 +672,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1023,8 +931,8 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1053,15 +961,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1075,9 +979,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1085,37 +986,47 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1131,17 +1042,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1363,10 +1271,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B3:I1005"/>
+  <dimension ref="B3:I1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1380,67 +1288,67 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B3" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
+      <c r="B3" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
+      <c r="B4" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="43">
+      <c r="B5" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="31">
         <v>44086</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="44">
+      <c r="B6" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="32">
         <v>44089</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="B7" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37" t="s">
+      <c r="B8" s="37"/>
+      <c r="C8" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -1480,29 +1388,29 @@
       </c>
     </row>
     <row r="11" spans="2:9" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="7">
         <v>1</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="G11" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="I11" s="43" t="s">
         <v>12</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="28" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
@@ -1510,448 +1418,390 @@
       <c r="C12" s="7">
         <v>2</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F12" s="11" t="s">
+      <c r="H12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="I12" s="43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B13" s="40" t="s">
         <v>17</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B13" s="39" t="s">
-        <v>19</v>
       </c>
       <c r="C13" s="7">
         <v>3</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="H13" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="28" t="s">
-        <v>14</v>
+      <c r="I13" s="43" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="40"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="7">
         <v>4</v>
       </c>
-      <c r="D14" s="31" t="s">
-        <v>24</v>
+      <c r="D14" s="27" t="s">
+        <v>22</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="43" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B15" s="40"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="7">
         <v>5</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="9" t="s">
+      <c r="H15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="408" x14ac:dyDescent="0.2">
-      <c r="B16" s="13"/>
+      <c r="I15" s="43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B16" s="29"/>
       <c r="C16" s="7">
         <v>6</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="13"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B18" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="7">
+        <v>7</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F16" s="9" t="s">
+      <c r="F18" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="408" x14ac:dyDescent="0.2">
-      <c r="B17" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="7">
-        <v>7</v>
-      </c>
-      <c r="D17" s="31" t="s">
+    </row>
+    <row r="19" spans="2:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="B19" s="34"/>
+      <c r="C19" s="7">
+        <v>8</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="9" t="s">
+      <c r="F19" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B18" s="34"/>
-      <c r="C18" s="7">
-        <v>8</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="I18" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="15"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B20" s="41" t="s">
-        <v>90</v>
-      </c>
+    </row>
+    <row r="20" spans="2:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="B20" s="29"/>
       <c r="C20" s="7">
         <v>9</v>
       </c>
-      <c r="D20" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="9" t="s">
+      <c r="D20" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H20" s="12" t="s">
+      <c r="E20" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="28" t="s">
-        <v>14</v>
+      <c r="F20" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="43" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B21" s="34"/>
+      <c r="B21" s="33" t="s">
+        <v>79</v>
+      </c>
       <c r="C21" s="7">
         <v>10</v>
       </c>
-      <c r="D21" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="H21" s="12" t="s">
+      <c r="D21" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I21" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" ht="395.25" x14ac:dyDescent="0.2">
-      <c r="B22" s="33" t="s">
-        <v>93</v>
-      </c>
+      <c r="F21" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="B22" s="34"/>
       <c r="C22" s="7">
         <v>11</v>
       </c>
-      <c r="D22" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="16" t="s">
+      <c r="D22" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I22" s="28" t="s">
-        <v>14</v>
+      <c r="I22" s="43" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B23" s="34"/>
+      <c r="B23" s="35" t="s">
+        <v>82</v>
+      </c>
       <c r="C23" s="7">
         <v>12</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="I23" s="28" t="s">
-        <v>14</v>
+      <c r="I23" s="43" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B24" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="B24" s="34"/>
       <c r="C24" s="7">
         <v>13</v>
       </c>
-      <c r="D24" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="12" t="s">
+      <c r="D24" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="B25" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I24" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B25" s="34"/>
       <c r="C25" s="7">
         <v>14</v>
       </c>
-      <c r="D25" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="H25" s="12" t="s">
+      <c r="D25" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I25" s="43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B26" s="16" t="s">
         <v>52</v>
-      </c>
-      <c r="I25" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B26" s="45" t="s">
-        <v>97</v>
       </c>
       <c r="C26" s="7">
         <v>15</v>
       </c>
-      <c r="D26" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="E26" s="12" t="s">
+      <c r="D26" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="I26" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B27" s="34"/>
-      <c r="C27" s="7">
-        <v>16</v>
-      </c>
-      <c r="D27" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="I27" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B28" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="7">
-        <v>17</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="I28" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B29" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="7">
-        <v>18</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="I29" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="20"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="23"/>
+      <c r="I26" s="43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="28" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D31" s="1"/>
@@ -2034,20 +1884,14 @@
     <row r="44" spans="4:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="4:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
     </row>
     <row r="46" spans="4:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D46" s="1"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
     </row>
     <row r="47" spans="4:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D47" s="1"/>
@@ -5873,56 +5717,39 @@
       <c r="D1002" s="1"/>
       <c r="F1002" s="1"/>
     </row>
-    <row r="1003" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D1003" s="1"/>
-      <c r="F1003" s="1"/>
-    </row>
-    <row r="1004" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D1004" s="1"/>
-      <c r="F1004" s="1"/>
-    </row>
-    <row r="1005" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D1005" s="1"/>
-      <c r="F1005" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
+  <mergeCells count="12">
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="G11" r:id="rId2" display="Display following information of the given CSV file in the CLI_x000a__x000a_number of fruits:_x000a_Total types of fruits:_x000a_Oldest fruit &amp; age:_x000a_The number of each type of fruit in descending order:_x000a_The various characteristics (count, color, shape, etc.) of each fruit by typ" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="F12" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="F15" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F16" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F17" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E18" r:id="rId7" display="1. Open the test.CSV file_x000a_2. Remove one column from the data._x000a_3. Upload the file._x000a_4. Set the correct uploaded path to the &quot;filepath&quot; variable and set the file name to the &quot;filename&quot; variable._x000a_5 Execute the fruitbasketapp.sh script." xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F23" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F24" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F25" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F26" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="F27" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="F28" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="F29" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F18" r:id="rId18" xr:uid="{32F165F6-CC11-4E22-8059-215905F9F3FD}"/>
+    <hyperlink ref="E16" r:id="rId5" display="1. Open the test.CSV file_x000a_2. Remove one column from the data._x000a_3. Upload the file._x000a_4. Set the correct uploaded path to the &quot;filepath&quot; variable and set the file name to the &quot;filename&quot; variable._x000a_5 Execute the fruitbasketapp.sh script." xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F18" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F19" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F23" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F24" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F25" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F26" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{32F165F6-CC11-4E22-8059-215905F9F3FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId19"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>